<commit_message>
The budget is ready i think
</commit_message>
<xml_diff>
--- a/Budget/Budget.xlsx
+++ b/Budget/Budget.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="77">
   <si>
     <t xml:space="preserve">Item</t>
   </si>
@@ -238,7 +238,7 @@
     <t xml:space="preserve">LM2576S-3.3</t>
   </si>
   <si>
-    <t xml:space="preserve">Inductor grande xd</t>
+    <t xml:space="preserve">EA77-625</t>
   </si>
   <si>
     <t xml:space="preserve">Quote</t>
@@ -543,8 +543,8 @@
   </sheetPr>
   <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D24" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G45" activeCellId="0" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1202,7 +1202,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="n">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>38</v>
@@ -1228,21 +1228,21 @@
       </c>
       <c r="J14" s="3" t="n">
         <f aca="false">B14*2</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K14" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L14" s="5" t="n">
         <f aca="false">J14-K14</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>28</v>
       </c>
       <c r="N14" s="4" t="n">
         <f aca="false">I14*J14</f>
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
@@ -2755,12 +2755,14 @@
         <v>24</v>
       </c>
       <c r="G45" s="4" t="n">
-        <v>3451</v>
-      </c>
-      <c r="H45" s="6"/>
+        <v>47600</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="I45" s="4" t="n">
         <f aca="false">G45</f>
-        <v>3451</v>
+        <v>47600</v>
       </c>
       <c r="J45" s="3" t="n">
         <f aca="false">B45*2</f>
@@ -2773,16 +2775,18 @@
         <f aca="false">J45-K45</f>
         <v>2</v>
       </c>
-      <c r="M45" s="3"/>
+      <c r="M45" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="N45" s="4" t="n">
         <f aca="false">I45*J45</f>
-        <v>6902</v>
+        <v>95200</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N46" s="10" t="n">
         <f aca="false">SUM(N2:N44)</f>
-        <v>662512.42</v>
+        <v>665512.42</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2794,7 +2798,7 @@
       </c>
       <c r="N47" s="12" t="n">
         <f aca="false">N46/7</f>
-        <v>94644.6314285714</v>
+        <v>95073.2028571428</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2813,7 +2817,7 @@
       <c r="H51" s="3"/>
       <c r="I51" s="14" t="n">
         <f aca="false">N$46/7</f>
-        <v>94644.6314285714</v>
+        <v>95073.2028571428</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2823,7 +2827,7 @@
       <c r="H52" s="3"/>
       <c r="I52" s="14" t="n">
         <f aca="false">N$46/7</f>
-        <v>94644.6314285714</v>
+        <v>95073.2028571428</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2833,7 +2837,7 @@
       <c r="H53" s="3"/>
       <c r="I53" s="14" t="n">
         <f aca="false">N$46/7</f>
-        <v>94644.6314285714</v>
+        <v>95073.2028571428</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2843,7 +2847,7 @@
       <c r="H54" s="15"/>
       <c r="I54" s="14" t="n">
         <f aca="false">N$46/7</f>
-        <v>94644.6314285714</v>
+        <v>95073.2028571428</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2853,7 +2857,7 @@
       <c r="H55" s="3"/>
       <c r="I55" s="14" t="n">
         <f aca="false">N$46/7</f>
-        <v>94644.6314285714</v>
+        <v>95073.2028571428</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2863,7 +2867,7 @@
       <c r="H56" s="3"/>
       <c r="I56" s="14" t="n">
         <f aca="false">N$46/7</f>
-        <v>94644.6314285714</v>
+        <v>95073.2028571428</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2873,7 +2877,7 @@
       <c r="H57" s="3"/>
       <c r="I57" s="14" t="n">
         <f aca="false">N$46/7</f>
-        <v>94644.6314285714</v>
+        <v>95073.2028571428</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some formating in the budget
</commit_message>
<xml_diff>
--- a/Budget/Budget.xlsx
+++ b/Budget/Budget.xlsx
@@ -786,15 +786,15 @@
   </sheetPr>
   <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O5" activeCellId="0" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="12.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.5"/>
@@ -2156,7 +2156,7 @@
         <v>12</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="N27" s="4" t="n">
         <f aca="false">I27*J27</f>
@@ -2207,7 +2207,7 @@
         <v>12</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="N28" s="4" t="n">
         <f aca="false">I28*J28</f>
@@ -2216,7 +2216,7 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="n">
         <f aca="false">A28+1</f>
         <v>28</v>
@@ -2258,7 +2258,7 @@
         <v>2</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="N29" s="4" t="n">
         <f aca="false">I29*J29</f>
@@ -2267,7 +2267,7 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="n">
         <f aca="false">A29+1</f>
         <v>29</v>
@@ -2309,7 +2309,7 @@
         <v>4</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="N30" s="4" t="n">
         <f aca="false">I30*J30</f>
@@ -2318,7 +2318,7 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="n">
         <f aca="false">A30+1</f>
         <v>30</v>
@@ -2360,7 +2360,7 @@
         <v>4</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="N31" s="4" t="n">
         <f aca="false">I31*J31</f>
@@ -2369,7 +2369,7 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="n">
         <f aca="false">A31+1</f>
         <v>31</v>
@@ -2411,7 +2411,7 @@
         <v>6</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="N32" s="4" t="n">
         <f aca="false">I32*J32</f>
@@ -2420,7 +2420,7 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="n">
         <f aca="false">A32+1</f>
         <v>32</v>
@@ -2462,7 +2462,7 @@
         <v>12</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="N33" s="4" t="n">
         <f aca="false">I33*J33</f>

</xml_diff>